<commit_message>
implementado forma de retirada de equipamentos, telinha de loguin foi estilizada,mensagens de aviso desnecessarias foram retiradas, forma de apagar os equipamentos retirados foram criadas, alem disso o usuario master poderá apagar o historico de peças retiradas, controle de acesso a determinados pontos do sistema foram melhorados
</commit_message>
<xml_diff>
--- a/Rotina de testes.xlsx
+++ b/Rotina de testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\repositorios\controle de estoque bilhetagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66321BEB-E0C0-473F-A4C3-F7B8B90E0AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CA207F-F542-4EFB-875C-3DC7C2248C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>logar com usuario verificar se esta logando corretamente</t>
   </si>
@@ -51,9 +51,6 @@
     <t>tentar visualizar o estoque deslogado</t>
   </si>
   <si>
-    <t>esta funcionando corretamente</t>
-  </si>
-  <si>
     <t xml:space="preserve">fazer uma retirada de equipamento deslogado </t>
   </si>
   <si>
@@ -84,19 +81,31 @@
     <t>funcionando corretamente</t>
   </si>
   <si>
-    <t>mostrando mesmo conteudo para entradas e saidas, antes estava funcionando normal</t>
-  </si>
-  <si>
-    <t>considerando equipamentos  assim informando duplicatas</t>
-  </si>
-  <si>
-    <t>não realiza, mas precisa informar o usuario</t>
-  </si>
-  <si>
-    <t>funciona como esperado</t>
-  </si>
-  <si>
-    <t>não autoriza, como esperado</t>
+    <t>não realiza a retirada, mas não informa isso ao usuario, dando a entender que realizou</t>
+  </si>
+  <si>
+    <t>mesma situação de quando se tenta fazer saida de equipamento deslogado</t>
+  </si>
+  <si>
+    <t>informa que não é autorizado</t>
+  </si>
+  <si>
+    <t>não é autorizado conforme esperado</t>
+  </si>
+  <si>
+    <t>logando corretamente?</t>
+  </si>
+  <si>
+    <t>ok logando com sucesso</t>
+  </si>
+  <si>
+    <t>ok funcionando corretamente</t>
+  </si>
+  <si>
+    <t>ok delogando corretamente</t>
+  </si>
+  <si>
+    <t>não realiza o loguin conforme esperado</t>
   </si>
 </sst>
 </file>
@@ -440,7 +449,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -479,8 +488,8 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,7 +511,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -521,10 +530,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,10 +541,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,10 +552,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -554,10 +563,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,10 +596,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,10 +607,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,10 +618,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,10 +629,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,18 +640,22 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">

</xml_diff>

<commit_message>
Bugs de loguin corrigidos, melhora consideravel no layout da pagina do sistema
</commit_message>
<xml_diff>
--- a/Rotina de testes.xlsx
+++ b/Rotina de testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\repositorios\controle de estoque bilhetagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CA207F-F542-4EFB-875C-3DC7C2248C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C94A9D3-A7B2-49F1-B17E-DC698FCE8BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>logar com usuario verificar se esta logando corretamente</t>
   </si>
@@ -33,9 +33,6 @@
     <t>fazer logout, verificar se o usuario foi mesmo deslogado</t>
   </si>
   <si>
-    <t>acessar inserção de novos equipamentos deslogado</t>
-  </si>
-  <si>
     <t>acessar inserção de novos equipamentos logado</t>
   </si>
   <si>
@@ -78,41 +75,74 @@
     <t>verificar deslogar</t>
   </si>
   <si>
-    <t>funcionando corretamente</t>
-  </si>
-  <si>
-    <t>não realiza a retirada, mas não informa isso ao usuario, dando a entender que realizou</t>
-  </si>
-  <si>
-    <t>mesma situação de quando se tenta fazer saida de equipamento deslogado</t>
-  </si>
-  <si>
-    <t>informa que não é autorizado</t>
-  </si>
-  <si>
-    <t>não é autorizado conforme esperado</t>
-  </si>
-  <si>
-    <t>logando corretamente?</t>
-  </si>
-  <si>
-    <t>ok logando com sucesso</t>
-  </si>
-  <si>
-    <t>ok funcionando corretamente</t>
-  </si>
-  <si>
-    <t>ok delogando corretamente</t>
-  </si>
-  <si>
-    <t>não realiza o loguin conforme esperado</t>
+    <t>não loga com senha incorreta</t>
+  </si>
+  <si>
+    <t>não loga com email errado</t>
+  </si>
+  <si>
+    <t>mensagem de usuario não autorizado</t>
+  </si>
+  <si>
+    <t>sim o usuario esta sendo deslogado quando faz logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">não realiza a retirada, mas informa que foi retirada </t>
+  </si>
+  <si>
+    <t>informa que teve sucesso, mesmo não tendo sido realizada a operação</t>
+  </si>
+  <si>
+    <t>tela de loguin ok</t>
+  </si>
+  <si>
+    <t>não loga com senha ou email incorretas</t>
+  </si>
+  <si>
+    <t>ok esta realizando as entradas com sucesso</t>
+  </si>
+  <si>
+    <t>ok esta realizando as saidas com sucesso</t>
+  </si>
+  <si>
+    <t>deslogando com sucesso</t>
+  </si>
+  <si>
+    <t>inserindo corretamente</t>
+  </si>
+  <si>
+    <t>realizando corretamente</t>
+  </si>
+  <si>
+    <t>esta logando corretamente</t>
+  </si>
+  <si>
+    <t>criar um novo equipamento com usuario não autorizado</t>
+  </si>
+  <si>
+    <t>visualizar estoque com usuario não autorizado</t>
+  </si>
+  <si>
+    <t>apesar de não inserir o equipamento, o sistema informa que o procedimento foi realizdo</t>
+  </si>
+  <si>
+    <t>visualiza corretamente</t>
+  </si>
+  <si>
+    <t>está acessando, preciso corrigir isso o mais rapido possivel</t>
+  </si>
+  <si>
+    <t>tela master</t>
+  </si>
+  <si>
+    <t>não esta limpando os campos de texto quando cria novo usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +152,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,10 +207,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,265 +493,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
-    <col min="3" max="3" width="81.5703125" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="86.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>20</v>
-      </c>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nessa versão apenas usuarios autorizados tem acesso a diversas partes do sistema, tambem tivemos a especificação de usuarios, de forma que caso o usuario não tenha acesso a determinada parte do banco de dados, ele tambem não vai conseguir acessar a funcionalidade do sistema
</commit_message>
<xml_diff>
--- a/Rotina de testes.xlsx
+++ b/Rotina de testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\repositorios\controle de estoque bilhetagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C94A9D3-A7B2-49F1-B17E-DC698FCE8BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E260248C-BB5F-48A3-A350-3D5B043C3C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,124 +25,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
-  <si>
-    <t>logar com usuario verificar se esta logando corretamente</t>
-  </si>
-  <si>
-    <t>fazer logout, verificar se o usuario foi mesmo deslogado</t>
-  </si>
-  <si>
-    <t>acessar inserção de novos equipamentos logado</t>
-  </si>
-  <si>
-    <t>tentar logar com senha errada</t>
-  </si>
-  <si>
-    <t>tentar logar com emai errado</t>
-  </si>
-  <si>
-    <t>tentar visualizar o estoque logado</t>
-  </si>
-  <si>
-    <t>tentar visualizar o estoque deslogado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fazer uma retirada de equipamento deslogado </t>
-  </si>
-  <si>
-    <t>fazer uma retirada de equipamento logado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fazer uma entrada de equipamento deslogado </t>
-  </si>
-  <si>
-    <t>fazer uma entrada de equipamento logado</t>
-  </si>
-  <si>
-    <t>verificar no aplicativo  loguin</t>
-  </si>
-  <si>
-    <t>verificar no app movel logar errado</t>
-  </si>
-  <si>
-    <t>verificar entrada de equipamento</t>
-  </si>
-  <si>
-    <t>verificar saida de equipamento</t>
-  </si>
-  <si>
-    <t>verificar deslogar</t>
-  </si>
-  <si>
-    <t>não loga com senha incorreta</t>
-  </si>
-  <si>
-    <t>não loga com email errado</t>
-  </si>
-  <si>
-    <t>mensagem de usuario não autorizado</t>
-  </si>
-  <si>
-    <t>sim o usuario esta sendo deslogado quando faz logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">não realiza a retirada, mas informa que foi retirada </t>
-  </si>
-  <si>
-    <t>informa que teve sucesso, mesmo não tendo sido realizada a operação</t>
-  </si>
-  <si>
-    <t>tela de loguin ok</t>
-  </si>
-  <si>
-    <t>não loga com senha ou email incorretas</t>
-  </si>
-  <si>
-    <t>ok esta realizando as entradas com sucesso</t>
-  </si>
-  <si>
-    <t>ok esta realizando as saidas com sucesso</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>deslogando com sucesso</t>
   </si>
   <si>
-    <t>inserindo corretamente</t>
-  </si>
-  <si>
-    <t>realizando corretamente</t>
-  </si>
-  <si>
-    <t>esta logando corretamente</t>
-  </si>
-  <si>
-    <t>criar um novo equipamento com usuario não autorizado</t>
-  </si>
-  <si>
-    <t>visualizar estoque com usuario não autorizado</t>
-  </si>
-  <si>
-    <t>apesar de não inserir o equipamento, o sistema informa que o procedimento foi realizdo</t>
-  </si>
-  <si>
-    <t>visualiza corretamente</t>
-  </si>
-  <si>
-    <t>está acessando, preciso corrigir isso o mais rapido possivel</t>
-  </si>
-  <si>
-    <t>tela master</t>
-  </si>
-  <si>
-    <t>não esta limpando os campos de texto quando cria novo usuario</t>
+    <t>logar no aplicativo mobile</t>
+  </si>
+  <si>
+    <t>logou com sucesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">realizar uma entrada </t>
+  </si>
+  <si>
+    <t>realizou entrada com sucesso</t>
+  </si>
+  <si>
+    <t>simular uma entrada duplicada(use o mesmo serial acima)</t>
+  </si>
+  <si>
+    <t>Não realiza a entrada, informa que a mesma já foi realizada anteriormente</t>
+  </si>
+  <si>
+    <t>dê saida nesse equipamento</t>
+  </si>
+  <si>
+    <t>realizou a saida do equipamento com sucesso</t>
+  </si>
+  <si>
+    <t>realizar uma saida duplicada</t>
+  </si>
+  <si>
+    <t>não realiza saida duplicada de equipamentos</t>
+  </si>
+  <si>
+    <t>realizar logout</t>
+  </si>
+  <si>
+    <t>realizar loguin desktop</t>
+  </si>
+  <si>
+    <t>realizou a entrada com sucesso</t>
+  </si>
+  <si>
+    <t>não realiza  entrada duplicada e informa que a mesma foi realizada anteriormente</t>
+  </si>
+  <si>
+    <t>não realiza saida duplicada de equipamentos pede para o usuario conferir o numero serial</t>
+  </si>
+  <si>
+    <t>acessar tela de inserção de equipamentos com usuario sem autorização</t>
+  </si>
+  <si>
+    <t>não permite acesso, caso desse acesso, o mesmo não conseguiria acessar e modificar os dados</t>
+  </si>
+  <si>
+    <t>acessar com usuario com autorização admin ou master</t>
+  </si>
+  <si>
+    <t>acesso realizado com sucesso</t>
+  </si>
+  <si>
+    <t>realizar uma entrada  duplicada (use o serial anterior)</t>
+  </si>
+  <si>
+    <t>realizar a saida do equipamento anterior</t>
+  </si>
+  <si>
+    <t>realizar saida duplicada do equipamento anteriro</t>
+  </si>
+  <si>
+    <t>não realiza a saida duplicada de equipamentos</t>
+  </si>
+  <si>
+    <t>acessar opção de inserção de novos equipamentos</t>
+  </si>
+  <si>
+    <t>não esta permitindo que o usuario master acesse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +119,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,16 +461,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66" customWidth="1"/>
     <col min="2" max="2" width="86.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -518,87 +478,87 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -606,55 +566,55 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>